<commit_message>
commit: 1. no cell data -> out
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\python_for_desk\bm_pd_summary_extractor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\python_for_desk\BM-PD_summary_all_site\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,43 +18,14 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="12" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
-  <si>
-    <t>날짜</t>
-  </si>
-  <si>
-    <t>종류</t>
-  </si>
-  <si>
-    <t>호기</t>
-  </si>
-  <si>
-    <t>공정</t>
-  </si>
-  <si>
-    <t>발생시간</t>
-  </si>
-  <si>
-    <t>조치완료</t>
-  </si>
-  <si>
-    <t>처리시간(분)</t>
-  </si>
-  <si>
-    <t>작업자</t>
-  </si>
-  <si>
-    <t>현상</t>
-  </si>
-  <si>
-    <t>조치</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>행 레이블</t>
   </si>
@@ -68,10 +39,59 @@
     <t>열 레이블</t>
   </si>
   <si>
-    <t>합계 : 처리시간(분)</t>
+    <t>개수 : 현상</t>
   </si>
   <si>
-    <t>개수 : 현상</t>
+    <t>0. Site</t>
+  </si>
+  <si>
+    <t>1. 호기</t>
+  </si>
+  <si>
+    <t>2-1. Machine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-2. Unit</t>
+  </si>
+  <si>
+    <t>2-3. Assy</t>
+  </si>
+  <si>
+    <t>3-1. 발생시간</t>
+  </si>
+  <si>
+    <t>3-2. 조치완료</t>
+  </si>
+  <si>
+    <t>4. 작업자</t>
+  </si>
+  <si>
+    <t>5. 현상</t>
+  </si>
+  <si>
+    <t>6. 원인</t>
+  </si>
+  <si>
+    <t>7. 조치</t>
+  </si>
+  <si>
+    <t>종류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>종류</t>
+  </si>
+  <si>
+    <t>(모두)</t>
+  </si>
+  <si>
+    <t>3-3. 조치 시간(분)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -136,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -145,7 +165,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -155,11 +174,329 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="39">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment vertical="center" readingOrder="0"/>
     </dxf>
@@ -357,56 +694,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color indexed="64"/>
@@ -466,7 +753,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="User" refreshedDate="45792.323349189814" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="281">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J1048576" sheet="RawData"/>
+    <worksheetSource ref="B1:L1048576" sheet="RawData"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="날짜" numFmtId="0">
@@ -582,6 +869,68 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="User" refreshedDate="45799.058131712962" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="1">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:N1048576" sheet="RawData"/>
+  </cacheSource>
+  <cacheFields count="13">
+    <cacheField name="날짜" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="종류" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="0. Site" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="1. 호기" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="2-1. Machine" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="2-2. Unit" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="2-3. Assy" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="3-1. 발생시간" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="3-2. 조치완료" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="4. 작업자" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="5. 현상" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="6. 원인" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="7. 조치" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="281">
   <r>
@@ -3949,6 +4298,26 @@
     <m/>
     <x v="0"/>
     <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
     <m/>
     <m/>
     <m/>
@@ -3960,106 +4329,47 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="8">
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="4"/>
-        <item m="1" x="3"/>
-        <item m="1" x="2"/>
-        <item m="1" x="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0">
+      <items count="2">
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="66">
-        <item m="1" x="6"/>
-        <item m="1" x="20"/>
-        <item m="1" x="63"/>
-        <item m="1" x="19"/>
-        <item m="1" x="59"/>
-        <item m="1" x="2"/>
-        <item m="1" x="43"/>
-        <item m="1" x="22"/>
-        <item m="1" x="13"/>
-        <item m="1" x="44"/>
-        <item m="1" x="58"/>
-        <item m="1" x="51"/>
-        <item m="1" x="52"/>
-        <item m="1" x="36"/>
-        <item m="1" x="56"/>
-        <item m="1" x="27"/>
-        <item m="1" x="34"/>
-        <item m="1" x="45"/>
-        <item m="1" x="53"/>
-        <item m="1" x="42"/>
-        <item m="1" x="21"/>
-        <item m="1" x="3"/>
-        <item m="1" x="18"/>
-        <item m="1" x="15"/>
-        <item m="1" x="38"/>
-        <item m="1" x="12"/>
-        <item m="1" x="35"/>
-        <item m="1" x="14"/>
-        <item m="1" x="17"/>
-        <item m="1" x="49"/>
-        <item m="1" x="10"/>
-        <item m="1" x="28"/>
-        <item m="1" x="23"/>
-        <item m="1" x="8"/>
-        <item m="1" x="1"/>
-        <item m="1" x="9"/>
-        <item m="1" x="39"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item m="1" x="41"/>
-        <item m="1" x="24"/>
-        <item m="1" x="32"/>
-        <item m="1" x="4"/>
-        <item m="1" x="61"/>
-        <item m="1" x="64"/>
-        <item m="1" x="57"/>
-        <item m="1" x="33"/>
-        <item m="1" x="26"/>
-        <item m="1" x="40"/>
-        <item m="1" x="37"/>
-        <item m="1" x="11"/>
-        <item m="1" x="50"/>
-        <item m="1" x="54"/>
-        <item m="1" x="16"/>
-        <item m="1" x="48"/>
-        <item m="1" x="25"/>
-        <item m="1" x="30"/>
-        <item m="1" x="47"/>
-        <item m="1" x="29"/>
-        <item m="1" x="31"/>
-        <item m="1" x="60"/>
-        <item m="1" x="62"/>
-        <item m="1" x="55"/>
-        <item m="1" x="46"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="2">
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
   <rowItems count="2">
     <i>
-      <x v="64"/>
+      <x/>
     </i>
     <i t="grand">
       <x/>
@@ -4070,116 +4380,21 @@
   </colFields>
   <colItems count="2">
     <i>
-      <x v="6"/>
+      <x/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="합계 : 처리시간(분)" fld="6" baseField="3" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="26">
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <formats count="2">
+    <format dxfId="38">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="50">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="9"/>
-            <x v="10"/>
-            <x v="11"/>
-            <x v="12"/>
-            <x v="13"/>
-            <x v="14"/>
-            <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
-            <x v="18"/>
-            <x v="19"/>
-            <x v="20"/>
-            <x v="21"/>
-            <x v="22"/>
-            <x v="23"/>
-            <x v="24"/>
-            <x v="25"/>
-            <x v="26"/>
-            <x v="27"/>
-            <x v="28"/>
-            <x v="29"/>
-            <x v="30"/>
-            <x v="31"/>
-            <x v="32"/>
-            <x v="33"/>
-            <x v="34"/>
-            <x v="35"/>
-            <x v="36"/>
-            <x v="37"/>
-            <x v="38"/>
-            <x v="39"/>
-            <x v="40"/>
-            <x v="41"/>
-            <x v="42"/>
-            <x v="43"/>
-            <x v="44"/>
-            <x v="45"/>
-            <x v="46"/>
-            <x v="47"/>
-            <x v="48"/>
-            <x v="49"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="15">
-            <x v="50"/>
-            <x v="51"/>
-            <x v="52"/>
-            <x v="53"/>
-            <x v="54"/>
-            <x v="55"/>
-            <x v="56"/>
-            <x v="57"/>
-            <x v="58"/>
-            <x v="59"/>
-            <x v="60"/>
-            <x v="61"/>
-            <x v="62"/>
-            <x v="63"/>
-            <x v="64"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="22">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="21">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -4192,7 +4407,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -4312,13 +4527,13 @@
     <dataField name="개수 : 현상" fld="8" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="21">
-    <format dxfId="20">
+    <format dxfId="36">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="35">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="50">
@@ -4376,7 +4591,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="15">
@@ -4399,26 +4614,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="29">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="28">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="50">
@@ -4476,7 +4691,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="15">
@@ -4499,26 +4714,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="22">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="21">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="50">
@@ -4576,7 +4791,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="15">
@@ -4599,17 +4814,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -4907,44 +5122,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11.875" customWidth="1"/>
+    <col min="5" max="7" width="20.625" customWidth="1"/>
+    <col min="8" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="16.625" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="17.625" customWidth="1"/>
+    <col min="14" max="14" width="22.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4955,16 +5191,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.75" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.25" bestFit="1" customWidth="1"/>
@@ -4975,36 +5208,41 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+      <c r="B1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
+      <c r="A4" s="2" t="s">
+        <v>0</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5032,38 +5270,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
+      <c r="A1" s="5" t="s">
+        <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>13</v>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>10</v>
+      <c r="A2" s="5" t="s">
+        <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>11</v>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>11</v>
+      <c r="A3" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
+      <c r="A4" s="6" t="s">
+        <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>